<commit_message>
v0.9.0 - Improved loading data function
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Design5\PycharmProjects\test.local.website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B669C34D-6184-4EDB-9226-600EF4D8C15B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBCD9C86-D518-4FF4-82AC-79D0971EAF9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="items" sheetId="1" r:id="rId1"/>
     <sheet name="models" sheetId="2" r:id="rId2"/>
+    <sheet name="book pricing" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
   <si>
     <t>Banner</t>
   </si>
@@ -52,24 +53,9 @@
     <t>Model</t>
   </si>
   <si>
-    <t>Roll-Up</t>
-  </si>
-  <si>
-    <t>Vinyl</t>
-  </si>
-  <si>
-    <t>Cardboard</t>
-  </si>
-  <si>
-    <t>Wooden</t>
-  </si>
-  <si>
     <t>Hardcover</t>
   </si>
   <si>
-    <t>Paperback</t>
-  </si>
-  <si>
     <t>Stamps</t>
   </si>
   <si>
@@ -83,13 +69,88 @@
   </si>
   <si>
     <t>S830</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Standard</t>
+  </si>
+  <si>
+    <t>Vinyl Banner</t>
+  </si>
+  <si>
+    <t>Small</t>
+  </si>
+  <si>
+    <t>Cardboard Box</t>
+  </si>
+  <si>
+    <t>Hardcover Book</t>
+  </si>
+  <si>
+    <t>Paperboard</t>
+  </si>
+  <si>
+    <t>300gsm Paper Box with flaps</t>
+  </si>
+  <si>
+    <t>Square Shape Stamp Size: 5x3CM</t>
+  </si>
+  <si>
+    <t>Square Shape Stamp Size: 6.4x4CM</t>
+  </si>
+  <si>
+    <t>Square Shape Stamp Size: 7.5x3.8CM</t>
+  </si>
+  <si>
+    <t>Square Shape Stamp Size: 6x3.5CM</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>A5</t>
+  </si>
+  <si>
+    <t>A6</t>
+  </si>
+  <si>
+    <t>B5</t>
+  </si>
+  <si>
+    <t>Books</t>
+  </si>
+  <si>
+    <t>Shields</t>
+  </si>
+  <si>
+    <t>binding type</t>
+  </si>
+  <si>
+    <t>binding cost</t>
+  </si>
+  <si>
+    <t>Saddle Stitch</t>
+  </si>
+  <si>
+    <t>Hard Cover</t>
+  </si>
+  <si>
+    <t>Spiral</t>
+  </si>
+  <si>
+    <t>Perfect Bound</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -99,6 +160,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -124,8 +193,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -406,10 +481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -431,12 +506,17 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -446,104 +526,247 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AED6BA6-BF74-47C2-A595-AA10F41F9B7D}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:B11"/>
+      <selection activeCell="A6" sqref="A6:A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.5703125" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
+    <col min="3" max="3" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="2">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="2">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="2">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="2">
+        <v>200</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7B5E229-6038-43C2-A7E8-BD3868DBF4B4}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
+        <v>32</v>
+      </c>
+      <c r="B3">
+        <v>2.5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
+        <v>35</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5">
         <v>15</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
v1.3.0 - fixed file reading, dataframes processing.
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
-  <workbookPr/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Design5\PycharmProjects\test.local.website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBCD9C86-D518-4FF4-82AC-79D0971EAF9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD7C057F-5802-49F9-90EE-F0B51B2EC1C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3585" yWindow="1440" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="items" sheetId="1" r:id="rId1"/>
@@ -36,26 +36,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
-  <si>
-    <t>Banner</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="36">
   <si>
     <t>Box</t>
   </si>
   <si>
-    <t>Book</t>
-  </si>
-  <si>
     <t>Item</t>
   </si>
   <si>
     <t>Model</t>
   </si>
   <si>
-    <t>Hardcover</t>
-  </si>
-  <si>
     <t>Stamps</t>
   </si>
   <si>
@@ -89,9 +80,6 @@
     <t>Cardboard Box</t>
   </si>
   <si>
-    <t>Hardcover Book</t>
-  </si>
-  <si>
     <t>Paperboard</t>
   </si>
   <si>
@@ -144,6 +132,18 @@
   </si>
   <si>
     <t>Perfect Bound</t>
+  </si>
+  <si>
+    <t>Banners</t>
+  </si>
+  <si>
+    <t>Sticker</t>
+  </si>
+  <si>
+    <t>Poster</t>
+  </si>
+  <si>
+    <t>Reflective</t>
   </si>
 </sst>
 </file>
@@ -481,42 +481,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -526,10 +527,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AED6BA6-BF74-47C2-A595-AA10F41F9B7D}">
-  <dimension ref="A1:D13"/>
+  <sheetPr codeName="Sheet2"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -542,172 +544,191 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D2" s="2">
-        <v>100</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D3" s="2">
         <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>5</v>
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D4" s="2">
-        <v>300</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D5" s="2">
-        <v>3</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D6" s="2">
-        <v>0.65</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D7" s="2">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D8" s="2">
-        <v>0.3</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>4</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="D9" s="2">
-        <v>0.5</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D10" s="2">
-        <v>120</v>
+        <v>140</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" t="s">
         <v>6</v>
       </c>
-      <c r="B11" t="s">
-        <v>8</v>
-      </c>
       <c r="C11" s="2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D11" s="2">
-        <v>140</v>
+        <v>180</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D12" s="2">
-        <v>180</v>
+        <v>200</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="B13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="D13" s="2">
-        <v>200</v>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="2">
+        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -718,25 +739,29 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7B5E229-6038-43C2-A7E8-BD3868DBF4B4}">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B2">
         <v>5</v>
@@ -744,7 +769,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B3">
         <v>2.5</v>
@@ -752,7 +777,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B4">
         <v>5</v>
@@ -760,7 +785,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B5">
         <v>15</v>

</xml_diff>

<commit_message>
v2.0.0 - multiple items table[Hs
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Design5\PycharmProjects\test.local.website\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Design5\Desktop\tagging\Versions\V2.0.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD7C057F-5802-49F9-90EE-F0B51B2EC1C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CC27330-F6CA-4AE2-B070-BF542DE4CFBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3585" yWindow="1440" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="180" yWindow="2400" windowWidth="21495" windowHeight="10785" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="items" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="36">
   <si>
     <t>Box</t>
   </si>
@@ -528,10 +528,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AED6BA6-BF74-47C2-A595-AA10F41F9B7D}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -729,6 +729,11 @@
       </c>
       <c r="D15" s="2">
         <v>180</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v2.1.0 - fixed adding items, added totals raw in the bottom of table
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Design5\Desktop\tagging\Versions\V2.0.1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Design5\PycharmProjects\test.local.website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CC27330-F6CA-4AE2-B070-BF542DE4CFBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD7C057F-5802-49F9-90EE-F0B51B2EC1C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="180" yWindow="2400" windowWidth="21495" windowHeight="10785" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3585" yWindow="1440" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="items" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="36">
   <si>
     <t>Box</t>
   </si>
@@ -528,10 +528,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AED6BA6-BF74-47C2-A595-AA10F41F9B7D}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -729,11 +729,6 @@
       </c>
       <c r="D15" s="2">
         <v>180</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>